<commit_message>
adding slide for meeting 11/16
</commit_message>
<xml_diff>
--- a/Research-Replay Data.xlsx
+++ b/Research-Replay Data.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27430"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="1220" yWindow="0" windowWidth="25600" windowHeight="15620" tabRatio="500"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Replay Application Observations</t>
   </si>
@@ -88,6 +88,18 @@
   </si>
   <si>
     <t>Netflix saves where you last left off in an episode, so difficult to replay if starting from the beginning</t>
+  </si>
+  <si>
+    <t>BBC News</t>
+  </si>
+  <si>
+    <t>Bubble Shoot</t>
+  </si>
+  <si>
+    <t>Color Note</t>
+  </si>
+  <si>
+    <t>Evernote</t>
   </si>
 </sst>
 </file>
@@ -225,6 +237,24 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -232,24 +262,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -583,35 +595,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:XFD13"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="14.5" style="6"/>
-    <col min="2" max="2" width="39.83203125" style="6" customWidth="1"/>
-    <col min="3" max="3" width="27" style="6" customWidth="1"/>
-    <col min="4" max="16384" width="14.5" style="6"/>
+    <col min="1" max="1" width="14.5" style="3"/>
+    <col min="2" max="2" width="39.83203125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="27" style="3" customWidth="1"/>
+    <col min="4" max="16384" width="14.5" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="13">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="5"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="11"/>
     </row>
     <row r="2" spans="1:3" ht="13">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="6" t="s">
         <v>3</v>
       </c>
     </row>
@@ -673,40 +685,93 @@
       </c>
     </row>
     <row r="10" spans="1:3" ht="24">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="7" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="24">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="24">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="11"/>
+      <c r="C12" s="8"/>
     </row>
     <row r="13" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A13" s="11"/>
-      <c r="B13" s="11"/>
-      <c r="C13" s="11"/>
+      <c r="A13" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+    </row>
+    <row r="14" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A14" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+    </row>
+    <row r="15" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A15" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+    </row>
+    <row r="16" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A16" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+    </row>
+    <row r="17" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A17" s="8"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+    </row>
+    <row r="18" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A18" s="8"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
+    </row>
+    <row r="19" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A19" s="8"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+    </row>
+    <row r="20" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A20" s="8"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
+    </row>
+    <row r="21" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A21" s="8"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+    </row>
+    <row r="22" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A22" s="8"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>